<commit_message>
Fixed offshore wind capacity figure. Also, fixed truncated data on CO2 emissions from the electricity sector.
</commit_message>
<xml_diff>
--- a/raw_data/offshore_wind_data.xlsx
+++ b/raw_data/offshore_wind_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wms5f/Programming/va_clean_economy_dashboard/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E03B83-7930-DE4C-933F-92BFB837F194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DDA396-7ABD-B04F-A839-C0DA2F2EB114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28700" windowHeight="17360" xr2:uid="{CBA4D054-97D9-4CDE-A24E-A0F5011C107D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31120" windowHeight="18180" xr2:uid="{CBA4D054-97D9-4CDE-A24E-A0F5011C107D}"/>
   </bookViews>
   <sheets>
     <sheet name="Offshore_wind_data" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="46">
   <si>
     <t>Total Production Forecast:</t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t>Total_mw</t>
+  </si>
+  <si>
+    <t>CVOW_Stage_I</t>
+  </si>
+  <si>
+    <t>CVOW_Stage_II</t>
+  </si>
+  <si>
+    <t>CVOW_Stage_III</t>
+  </si>
+  <si>
+    <t>CVOW_Pilot</t>
   </si>
 </sst>
 </file>
@@ -567,7 +579,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -604,16 +616,16 @@
         <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>31</v>
@@ -828,19 +840,19 @@
         <v>0</v>
       </c>
       <c r="K7" s="9">
-        <f>C7*$M$1*G7/100</f>
+        <f t="shared" ref="K7:K21" si="1">C7*$M$1*G7/100</f>
         <v>9460.7999999999993</v>
       </c>
       <c r="L7" s="9">
-        <f>D7*$M$1*H7/100</f>
+        <f t="shared" ref="L7:L21" si="2">D7*$M$1*H7/100</f>
         <v>0</v>
       </c>
       <c r="M7" s="9">
-        <f>E7*$M$1*I7/100</f>
+        <f t="shared" ref="M7:M21" si="3">E7*$M$1*I7/100</f>
         <v>0</v>
       </c>
       <c r="N7" s="9">
-        <f>F7*$M$1*J7/100</f>
+        <f t="shared" ref="N7:N21" si="4">F7*$M$1*J7/100</f>
         <v>0</v>
       </c>
       <c r="O7" s="9">
@@ -881,23 +893,23 @@
         <v>0</v>
       </c>
       <c r="K8" s="9">
-        <f>C8*$M$1*G8/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L8" s="9">
-        <f>D8*$M$1*H8/100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M8" s="9">
-        <f>E8*$M$1*I8/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N8" s="9">
-        <f>F8*$M$1*J8/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O8" s="9">
-        <f t="shared" ref="O8:O21" si="1">SUM(K8:N8)</f>
+        <f t="shared" ref="O8:O21" si="5">SUM(K8:N8)</f>
         <v>47093.760000000002</v>
       </c>
     </row>
@@ -934,23 +946,23 @@
         <v>0</v>
       </c>
       <c r="K9" s="9">
-        <f>C9*$M$1*G9/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L9" s="9">
-        <f>D9*$M$1*H9/100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M9" s="9">
-        <f>E9*$M$1*I9/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N9" s="9">
-        <f>F9*$M$1*J9/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O9" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>47093.760000000002</v>
       </c>
     </row>
@@ -987,23 +999,23 @@
         <v>0</v>
       </c>
       <c r="K10" s="9">
-        <f>C10*$M$1*G10/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L10" s="9">
-        <f>D10*$M$1*H10/100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M10" s="9">
-        <f>E10*$M$1*I10/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N10" s="9">
-        <f>F10*$M$1*J10/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>47093.760000000002</v>
       </c>
     </row>
@@ -1040,23 +1052,23 @@
         <v>0</v>
       </c>
       <c r="K11" s="9">
-        <f>C11*$M$1*G11/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L11" s="9">
-        <f>D11*$M$1*H11/100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M11" s="9">
-        <f>E11*$M$1*I11/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N11" s="9">
-        <f>F11*$M$1*J11/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>47093.760000000002</v>
       </c>
     </row>
@@ -1093,23 +1105,23 @@
         <v>0</v>
       </c>
       <c r="K12" s="9">
-        <f>C12*$M$1*G12/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L12" s="9">
-        <f>D12*$M$1*H12/100</f>
+        <f t="shared" si="2"/>
         <v>2721206.4</v>
       </c>
       <c r="M12" s="9">
-        <f>E12*$M$1*I12/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N12" s="9">
-        <f>F12*$M$1*J12/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O12" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2768300.1599999997</v>
       </c>
     </row>
@@ -1146,23 +1158,23 @@
         <v>35.299999999999997</v>
       </c>
       <c r="K13" s="9">
-        <f>C13*$M$1*G13/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L13" s="9">
-        <f>D13*$M$1*H13/100</f>
+        <f t="shared" si="2"/>
         <v>2883091.2</v>
       </c>
       <c r="M13" s="9">
-        <f>E13*$M$1*I13/100</f>
+        <f t="shared" si="3"/>
         <v>2721206.4</v>
       </c>
       <c r="N13" s="9">
-        <f>F13*$M$1*J13/100</f>
+        <f t="shared" si="4"/>
         <v>2721206.4</v>
       </c>
       <c r="O13" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8372597.7599999998</v>
       </c>
     </row>
@@ -1199,23 +1211,23 @@
         <v>37.4</v>
       </c>
       <c r="K14" s="9">
-        <f>C14*$M$1*G14/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L14" s="9">
-        <f>D14*$M$1*H14/100</f>
+        <f t="shared" si="2"/>
         <v>3044976</v>
       </c>
       <c r="M14" s="9">
-        <f>E14*$M$1*I14/100</f>
+        <f t="shared" si="3"/>
         <v>2883091.2</v>
       </c>
       <c r="N14" s="9">
-        <f>F14*$M$1*J14/100</f>
+        <f t="shared" si="4"/>
         <v>2883091.2</v>
       </c>
       <c r="O14" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8858252.1600000001</v>
       </c>
     </row>
@@ -1252,23 +1264,23 @@
         <v>39.4</v>
       </c>
       <c r="K15" s="9">
-        <f>C15*$M$1*G15/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L15" s="9">
-        <f>D15*$M$1*H15/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M15" s="9">
-        <f>E15*$M$1*I15/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N15" s="9">
-        <f>F15*$M$1*J15/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O15" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9158895.3599999994</v>
       </c>
     </row>
@@ -1305,23 +1317,23 @@
         <v>39.4</v>
       </c>
       <c r="K16" s="9">
-        <f>C16*$M$1*G16/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L16" s="9">
-        <f>D16*$M$1*H16/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M16" s="9">
-        <f>E16*$M$1*I16/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N16" s="9">
-        <f>F16*$M$1*J16/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O16" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9158895.3599999994</v>
       </c>
     </row>
@@ -1358,23 +1370,23 @@
         <v>39.4</v>
       </c>
       <c r="K17" s="9">
-        <f>C17*$M$1*G17/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L17" s="9">
-        <f>D17*$M$1*H17/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M17" s="9">
-        <f>E17*$M$1*I17/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N17" s="9">
-        <f>F17*$M$1*J17/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O17" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9158895.3599999994</v>
       </c>
     </row>
@@ -1411,23 +1423,23 @@
         <v>39.5</v>
       </c>
       <c r="K18" s="9">
-        <f>C18*$M$1*G18/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L18" s="9">
-        <f>D18*$M$1*H18/100</f>
+        <f t="shared" si="2"/>
         <v>3044976</v>
       </c>
       <c r="M18" s="9">
-        <f>E18*$M$1*I18/100</f>
+        <f t="shared" si="3"/>
         <v>3044976</v>
       </c>
       <c r="N18" s="9">
-        <f>F18*$M$1*J18/100</f>
+        <f t="shared" si="4"/>
         <v>3044976</v>
       </c>
       <c r="O18" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9182021.7599999998</v>
       </c>
     </row>
@@ -1464,23 +1476,23 @@
         <v>39.4</v>
       </c>
       <c r="K19" s="9">
-        <f>C19*$M$1*G19/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L19" s="9">
-        <f>D19*$M$1*H19/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M19" s="9">
-        <f>E19*$M$1*I19/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N19" s="9">
-        <f>F19*$M$1*J19/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O19" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9158895.3599999994</v>
       </c>
     </row>
@@ -1517,23 +1529,23 @@
         <v>39.4</v>
       </c>
       <c r="K20" s="9">
-        <f>C20*$M$1*G20/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L20" s="9">
-        <f>D20*$M$1*H20/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M20" s="9">
-        <f>E20*$M$1*I20/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N20" s="9">
-        <f>F20*$M$1*J20/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O20" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9158895.3599999994</v>
       </c>
     </row>
@@ -1570,23 +1582,23 @@
         <v>39.4</v>
       </c>
       <c r="K21" s="9">
-        <f>C21*$M$1*G21/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L21" s="9">
-        <f>D21*$M$1*H21/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M21" s="9">
-        <f>E21*$M$1*I21/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N21" s="9">
-        <f>F21*$M$1*J21/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9158895.3599999994</v>
       </c>
     </row>
@@ -1944,19 +1956,19 @@
         <v>0</v>
       </c>
       <c r="K7" s="9">
-        <f>C7*$M$1*G7/100</f>
+        <f t="shared" ref="K7:K21" si="1">C7*$M$1*G7/100</f>
         <v>9460.7999999999993</v>
       </c>
       <c r="L7" s="9">
-        <f>D7*$M$1*H7/100</f>
+        <f t="shared" ref="L7:L21" si="2">D7*$M$1*H7/100</f>
         <v>0</v>
       </c>
       <c r="M7" s="9">
-        <f>E7*$M$1*I7/100</f>
+        <f t="shared" ref="M7:M21" si="3">E7*$M$1*I7/100</f>
         <v>0</v>
       </c>
       <c r="N7" s="9">
-        <f>F7*$M$1*J7/100</f>
+        <f t="shared" ref="N7:N21" si="4">F7*$M$1*J7/100</f>
         <v>0</v>
       </c>
       <c r="O7" s="2"/>
@@ -2005,19 +2017,19 @@
         <v>0</v>
       </c>
       <c r="K8" s="9">
-        <f>C8*$M$1*G8/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L8" s="9">
-        <f>D8*$M$1*H8/100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M8" s="9">
-        <f>E8*$M$1*I8/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N8" s="9">
-        <f>F8*$M$1*J8/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O8" s="2"/>
@@ -2066,19 +2078,19 @@
         <v>0</v>
       </c>
       <c r="K9" s="9">
-        <f>C9*$M$1*G9/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L9" s="9">
-        <f>D9*$M$1*H9/100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M9" s="9">
-        <f>E9*$M$1*I9/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N9" s="9">
-        <f>F9*$M$1*J9/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O9" s="2"/>
@@ -2127,19 +2139,19 @@
         <v>0</v>
       </c>
       <c r="K10" s="9">
-        <f>C10*$M$1*G10/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L10" s="9">
-        <f>D10*$M$1*H10/100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M10" s="9">
-        <f>E10*$M$1*I10/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N10" s="9">
-        <f>F10*$M$1*J10/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O10" s="2"/>
@@ -2188,19 +2200,19 @@
         <v>0</v>
       </c>
       <c r="K11" s="9">
-        <f>C11*$M$1*G11/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L11" s="9">
-        <f>D11*$M$1*H11/100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M11" s="9">
-        <f>E11*$M$1*I11/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N11" s="9">
-        <f>F11*$M$1*J11/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O11" s="2"/>
@@ -2249,19 +2261,19 @@
         <v>0</v>
       </c>
       <c r="K12" s="9">
-        <f>C12*$M$1*G12/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L12" s="9">
-        <f>D12*$M$1*H12/100</f>
+        <f t="shared" si="2"/>
         <v>2721206.4</v>
       </c>
       <c r="M12" s="9">
-        <f>E12*$M$1*I12/100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N12" s="9">
-        <f>F12*$M$1*J12/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O12" s="2"/>
@@ -2310,19 +2322,19 @@
         <v>35.299999999999997</v>
       </c>
       <c r="K13" s="9">
-        <f>C13*$M$1*G13/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L13" s="9">
-        <f>D13*$M$1*H13/100</f>
+        <f t="shared" si="2"/>
         <v>2883091.2</v>
       </c>
       <c r="M13" s="9">
-        <f>E13*$M$1*I13/100</f>
+        <f t="shared" si="3"/>
         <v>2721206.4</v>
       </c>
       <c r="N13" s="9">
-        <f>F13*$M$1*J13/100</f>
+        <f t="shared" si="4"/>
         <v>2721206.4</v>
       </c>
       <c r="O13" s="2"/>
@@ -2371,19 +2383,19 @@
         <v>37.4</v>
       </c>
       <c r="K14" s="9">
-        <f>C14*$M$1*G14/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L14" s="9">
-        <f>D14*$M$1*H14/100</f>
+        <f t="shared" si="2"/>
         <v>3044976</v>
       </c>
       <c r="M14" s="9">
-        <f>E14*$M$1*I14/100</f>
+        <f t="shared" si="3"/>
         <v>2883091.2</v>
       </c>
       <c r="N14" s="9">
-        <f>F14*$M$1*J14/100</f>
+        <f t="shared" si="4"/>
         <v>2883091.2</v>
       </c>
       <c r="O14" s="2"/>
@@ -2432,19 +2444,19 @@
         <v>39.4</v>
       </c>
       <c r="K15" s="9">
-        <f>C15*$M$1*G15/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L15" s="9">
-        <f>D15*$M$1*H15/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M15" s="9">
-        <f>E15*$M$1*I15/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N15" s="9">
-        <f>F15*$M$1*J15/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O15" s="2"/>
@@ -2493,19 +2505,19 @@
         <v>39.4</v>
       </c>
       <c r="K16" s="9">
-        <f>C16*$M$1*G16/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L16" s="9">
-        <f>D16*$M$1*H16/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M16" s="9">
-        <f>E16*$M$1*I16/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N16" s="9">
-        <f>F16*$M$1*J16/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O16" s="2"/>
@@ -2554,19 +2566,19 @@
         <v>39.4</v>
       </c>
       <c r="K17" s="9">
-        <f>C17*$M$1*G17/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L17" s="9">
-        <f>D17*$M$1*H17/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M17" s="9">
-        <f>E17*$M$1*I17/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N17" s="9">
-        <f>F17*$M$1*J17/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O17" s="2"/>
@@ -2615,19 +2627,19 @@
         <v>39.5</v>
       </c>
       <c r="K18" s="9">
-        <f>C18*$M$1*G18/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L18" s="9">
-        <f>D18*$M$1*H18/100</f>
+        <f t="shared" si="2"/>
         <v>3044976</v>
       </c>
       <c r="M18" s="9">
-        <f>E18*$M$1*I18/100</f>
+        <f t="shared" si="3"/>
         <v>3044976</v>
       </c>
       <c r="N18" s="9">
-        <f>F18*$M$1*J18/100</f>
+        <f t="shared" si="4"/>
         <v>3044976</v>
       </c>
       <c r="O18" s="2"/>
@@ -2676,19 +2688,19 @@
         <v>39.4</v>
       </c>
       <c r="K19" s="9">
-        <f>C19*$M$1*G19/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L19" s="9">
-        <f>D19*$M$1*H19/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M19" s="9">
-        <f>E19*$M$1*I19/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N19" s="9">
-        <f>F19*$M$1*J19/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O19" s="2"/>
@@ -2737,19 +2749,19 @@
         <v>39.4</v>
       </c>
       <c r="K20" s="9">
-        <f>C20*$M$1*G20/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L20" s="9">
-        <f>D20*$M$1*H20/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M20" s="9">
-        <f>E20*$M$1*I20/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N20" s="9">
-        <f>F20*$M$1*J20/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O20" s="2"/>
@@ -2798,19 +2810,19 @@
         <v>39.4</v>
       </c>
       <c r="K21" s="9">
-        <f>C21*$M$1*G21/100</f>
+        <f t="shared" si="1"/>
         <v>47093.760000000002</v>
       </c>
       <c r="L21" s="9">
-        <f>D21*$M$1*H21/100</f>
+        <f t="shared" si="2"/>
         <v>3037267.2</v>
       </c>
       <c r="M21" s="9">
-        <f>E21*$M$1*I21/100</f>
+        <f t="shared" si="3"/>
         <v>3037267.2</v>
       </c>
       <c r="N21" s="9">
-        <f>F21*$M$1*J21/100</f>
+        <f t="shared" si="4"/>
         <v>3037267.2</v>
       </c>
       <c r="O21" s="2"/>

</xml_diff>